<commit_message>
Added comments to input_paramter files, for better readability.
Code cleanup.
</commit_message>
<xml_diff>
--- a/src/input_parameters.xlsx
+++ b/src/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="1380" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="10880" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,62 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>sigma min</t>
+  </si>
+  <si>
+    <t>amplitude</t>
+  </si>
+  <si>
+    <t>ampl. Min</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D3a</t>
+  </si>
+  <si>
+    <t>D3b</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>activate peak</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>fraction min</t>
+  </si>
+  <si>
+    <t>fraction max</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,218 +462,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1100</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>1250</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>1330</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>1420</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>1500</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>1590</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>1680</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>45</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>45</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <v>80</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>40</v>
       </c>
-      <c r="E3">
+      <c r="F4">
         <v>40</v>
       </c>
-      <c r="F3">
+      <c r="G4">
         <v>40</v>
       </c>
-      <c r="G3">
+      <c r="H4">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>40</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <v>40</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>40</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="G5">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H5">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <v>500</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>1000</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>5000</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>300</v>
       </c>
-      <c r="E5">
+      <c r="F6">
         <v>300</v>
       </c>
-      <c r="F5">
+      <c r="G6">
         <v>2000</v>
       </c>
-      <c r="G5">
+      <c r="H6">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
         <v>0.5</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <v>0.5</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>0.5</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <v>0.5</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>0.5</v>
       </c>
-      <c r="F7">
+      <c r="G8">
         <v>0.5</v>
       </c>
-      <c r="G7">
+      <c r="H8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>1</v>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added possibility to include max/min for any paramter.
</commit_message>
<xml_diff>
--- a/src/input_parameters.xlsx
+++ b/src/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="19980" yWindow="740" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>center</t>
   </si>
@@ -33,9 +33,6 @@
     <t>amplitude</t>
   </si>
   <si>
-    <t>ampl. Min</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
@@ -70,6 +67,21 @@
   </si>
   <si>
     <t>fraction max</t>
+  </si>
+  <si>
+    <t>center min</t>
+  </si>
+  <si>
+    <t>center max</t>
+  </si>
+  <si>
+    <t>sigma max</t>
+  </si>
+  <si>
+    <t>ampl. min</t>
+  </si>
+  <si>
+    <t>ampl. max</t>
   </si>
 </sst>
 </file>
@@ -118,8 +130,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,11 +142,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -475,33 +491,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -553,183 +569,203 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>45</v>
-      </c>
-      <c r="C4">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="E4">
-        <v>40</v>
-      </c>
-      <c r="F4">
-        <v>40</v>
-      </c>
-      <c r="G4">
-        <v>40</v>
-      </c>
-      <c r="H4">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>500</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>45</v>
       </c>
       <c r="D6">
-        <v>5000</v>
+        <v>80</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>2000</v>
+        <v>40</v>
       </c>
       <c r="H6">
-        <v>300</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0.5</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="D8">
-        <v>0.5</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <v>0.5</v>
-      </c>
-      <c r="G8">
-        <v>0.5</v>
-      </c>
-      <c r="H8">
-        <v>0.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added sigma_max to input parameters.
</commit_message>
<xml_diff>
--- a/src/input_parameters.xlsx
+++ b/src/input_parameters.xlsx
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -645,10 +645,25 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
       <c r="E8">
         <v>50</v>
       </c>
       <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New input parameter with extra peak.
This is not yet included in the self-creating script in multipeak.py
Will merge once it is more stable.
</commit_message>
<xml_diff>
--- a/src/input_parameters.xlsx
+++ b/src/input_parameters.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>center</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>ampl. max</t>
+  </si>
+  <si>
+    <t>init</t>
   </si>
 </sst>
 </file>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -489,7 +492,7 @@
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -514,8 +517,11 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -540,8 +546,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -566,8 +575,11 @@
       <c r="H3">
         <v>1680</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -578,7 +590,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -589,7 +601,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -614,8 +626,11 @@
       <c r="H6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -640,8 +655,11 @@
       <c r="H7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -666,8 +684,11 @@
       <c r="H8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -692,8 +713,11 @@
       <c r="H9">
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -718,13 +742,16 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -749,8 +776,11 @@
       <c r="H12">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -775,8 +805,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -799,6 +832,9 @@
         <v>1</v>
       </c>
       <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial fitting intensities are adjusted to the max of the spectral intensity
As a consequence, amplitudes in input_parameters.xlsx are expressed in
terms of relative rations of each peak.

This requires the amplitudes in older imput_parameters.xlsx to be changed
in order to be compatible with the new version of multifit.

Also, the initial fitting curve can be plotted or not through a flag at the
beginning of the script.
</commit_message>
<xml_diff>
--- a/src/input_parameters.xlsx
+++ b/src/input_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="22800" yWindow="1640" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>center</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>ampl. max</t>
-  </si>
-  <si>
-    <t>init</t>
   </si>
 </sst>
 </file>
@@ -133,8 +130,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,13 +144,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -492,7 +493,7 @@
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -517,11 +518,8 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -546,11 +544,8 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -575,33 +570,24 @@
       <c r="H3">
         <v>1680</v>
       </c>
-      <c r="I3">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="C4">
         <v>1240</v>
       </c>
-      <c r="F4">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="C5">
         <v>1275</v>
       </c>
-      <c r="E5">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -626,11 +612,8 @@
       <c r="H6">
         <v>40</v>
       </c>
-      <c r="I6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -655,11 +638,8 @@
       <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -684,40 +664,34 @@
       <c r="H8">
         <v>50</v>
       </c>
-      <c r="I8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
-        <v>500</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
-        <v>1000</v>
+        <v>0.2</v>
       </c>
       <c r="D9">
-        <v>5000</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>500</v>
+        <v>0.1</v>
       </c>
       <c r="F9">
-        <v>500</v>
+        <v>0.1</v>
       </c>
       <c r="G9">
-        <v>2000</v>
+        <v>0.8</v>
       </c>
       <c r="H9">
-        <v>300</v>
-      </c>
-      <c r="I9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -742,16 +716,13 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -776,11 +747,8 @@
       <c r="H12">
         <v>0.5</v>
       </c>
-      <c r="I12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -805,11 +773,8 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -832,9 +797,6 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
         <v>1</v>
       </c>
     </row>

</xml_diff>